<commit_message>
backup before deadline cleaning
</commit_message>
<xml_diff>
--- a/gams/python/results/Q1/res_sum_Q_in_RL.xlsx
+++ b/gams/python/results/Q1/res_sum_Q_in_RL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\CloudDrive\Uni\WS24\Research Project\gams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAFC8D4-1345-440D-B869-43370E0D5CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97677429-8725-4CD1-9B1D-16981F44DF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10665" yWindow="2520" windowWidth="7500" windowHeight="6000" xr2:uid="{3D9C1E58-DC0D-4571-905E-FECD64F2BF57}"/>
+    <workbookView xWindow="4180" yWindow="4180" windowWidth="28800" windowHeight="15460" xr2:uid="{3D9C1E58-DC0D-4571-905E-FECD64F2BF57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>